<commit_message>
parte inicial da revisao completada
</commit_message>
<xml_diff>
--- a/ficha conceitos-artigos.xlsx
+++ b/ficha conceitos-artigos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Artigos</t>
   </si>
@@ -76,28 +76,13 @@
     <t>Objeto de Aprendizado</t>
   </si>
   <si>
-    <t>Abordagem Inovadora</t>
-  </si>
-  <si>
-    <t>Gerenciamento.Negócio</t>
-  </si>
-  <si>
-    <t>Gerenciamento.Qualidade</t>
+    <t>Definição/Analogia de L.O</t>
   </si>
   <si>
     <t>Método Indutivo Ensino</t>
   </si>
   <si>
-    <t>Scrum</t>
-  </si>
-  <si>
-    <t>Analogia L.O</t>
-  </si>
-  <si>
     <t>Simuladores</t>
-  </si>
-  <si>
-    <t>Definição de L.O</t>
   </si>
   <si>
     <t>MRI</t>
@@ -120,7 +105,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -157,6 +142,7 @@
       <color rgb="FF00000A"/>
       <name val="arial"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -164,6 +150,7 @@
       <color rgb="FF00000A"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -171,6 +158,13 @@
       <color rgb="FF00000A"/>
       <name val="arial"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -255,7 +249,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,6 +292,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -385,9 +383,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.693023255814"/>
-    <col collapsed="false" hidden="false" max="22" min="3" style="0" width="3.69302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.693023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="22" min="3" style="0" width="3.81395348837209"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="12.0604651162791"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -551,13 +549,11 @@
       <c r="V5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -566,7 +562,9 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -579,14 +577,14 @@
       <c r="V6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -607,13 +605,11 @@
       <c r="V7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -621,9 +617,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -637,21 +631,20 @@
       <c r="V8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
@@ -665,13 +658,11 @@
       <c r="V9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -679,7 +670,9 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
@@ -693,10 +686,10 @@
       <c r="V10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -705,10 +698,10 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10" t="s">
+      <c r="K11" s="10" t="s">
         <v>15</v>
       </c>
+      <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
@@ -721,10 +714,10 @@
       <c r="V11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -734,7 +727,9 @@
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="L12" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -747,9 +742,7 @@
       <c r="V12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
@@ -760,9 +753,7 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -775,9 +766,7 @@
       <c r="V13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
@@ -787,9 +776,6 @@
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
@@ -803,9 +789,7 @@
       <c r="V14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
@@ -815,9 +799,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -831,9 +813,7 @@
       <c r="V15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
@@ -843,9 +823,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
@@ -859,9 +837,7 @@
       <c r="V16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>

</xml_diff>